<commit_message>
added php & csv format
</commit_message>
<xml_diff>
--- a/Nama-dan-Kode-Bank-Juni-2021.xlsx
+++ b/Nama-dan-Kode-Bank-Juni-2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\daftar-bank-di-indonesia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1AA48C29-432F-4D5D-9210-3228C330D21B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93D4C9E-99D9-4729-BCAC-57FE4666C4C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="285">
   <si>
     <t>Sandi Bank</t>
   </si>
@@ -687,9 +687,6 @@
     <t>BANK MESTIKA DHARMA</t>
   </si>
   <si>
-    <t>BANK WOORI</t>
-  </si>
-  <si>
     <t>BANK BUKOPIN</t>
   </si>
   <si>
@@ -798,15 +795,6 @@
     <t>BANK DKI</t>
   </si>
   <si>
-    <t>BANK DI YOGYAKARTA</t>
-  </si>
-  <si>
-    <t>BANK JAWA TENGAH</t>
-  </si>
-  <si>
-    <t>BANK BJAT</t>
-  </si>
-  <si>
     <t>BANK JAMBI</t>
   </si>
   <si>
@@ -828,24 +816,15 @@
     <t>BANK RIAU KEPRI</t>
   </si>
   <si>
-    <t>BANK SUMSEL DAN BABEL</t>
-  </si>
-  <si>
     <t>BANK SULSELBAR</t>
   </si>
   <si>
-    <t>BANK SULUT GORONTALO</t>
-  </si>
-  <si>
     <t>BANK KALSEL</t>
   </si>
   <si>
     <t>BANK KALBAR</t>
   </si>
   <si>
-    <t>BANK KALTIM DAN KALUT</t>
-  </si>
-  <si>
     <t>BANK KALTENG</t>
   </si>
   <si>
@@ -858,9 +837,6 @@
     <t>BANK NTT</t>
   </si>
   <si>
-    <t>BANK MALUKU DAN MALUKU UTARA</t>
-  </si>
-  <si>
     <t>BANK SULTENG</t>
   </si>
   <si>
@@ -883,6 +859,30 @@
   </si>
   <si>
     <t>NO.</t>
+  </si>
+  <si>
+    <t>BANK WOORI SAUDARA</t>
+  </si>
+  <si>
+    <t>BANK DI YOGYAKARTA (DIY)</t>
+  </si>
+  <si>
+    <t>BANK JATENG</t>
+  </si>
+  <si>
+    <t>BANK JATIM</t>
+  </si>
+  <si>
+    <t>BANK SUMSEL BABEL</t>
+  </si>
+  <si>
+    <t>BANK KALTARA</t>
+  </si>
+  <si>
+    <t>BANK SULUTGO</t>
+  </si>
+  <si>
+    <t>BANK MALUKU MALUT</t>
   </si>
 </sst>
 </file>
@@ -993,28 +993,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1292,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DEF08C-91E0-492F-BB6D-FCAFD7277C39}">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,10 +1286,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -1358,7 +1337,7 @@
         <v>183</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1439,7 +1418,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>134</v>
@@ -1691,7 +1670,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>219</v>
+        <v>277</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>121</v>
@@ -1719,7 +1698,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>122</v>
@@ -1733,7 +1712,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>123</v>
@@ -1747,7 +1726,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>124</v>
@@ -1761,7 +1740,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>125</v>
@@ -1775,7 +1754,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>126</v>
@@ -1789,7 +1768,7 @@
         <v>35</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D35" s="9">
         <v>498</v>
@@ -1803,7 +1782,7 @@
         <v>36</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>127</v>
@@ -1817,7 +1796,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>128</v>
@@ -1845,7 +1824,7 @@
         <v>39</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>143</v>
@@ -1873,7 +1852,7 @@
         <v>41</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>145</v>
@@ -1915,7 +1894,7 @@
         <v>44</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>148</v>
@@ -1929,7 +1908,7 @@
         <v>45</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>149</v>
@@ -1943,7 +1922,7 @@
         <v>46</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D46" s="9">
         <v>945</v>
@@ -1957,7 +1936,7 @@
         <v>47</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D47" s="9">
         <v>947</v>
@@ -1971,7 +1950,7 @@
         <v>48</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D48" s="9">
         <v>949</v>
@@ -2013,7 +1992,7 @@
         <v>51</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D51" s="9">
         <v>405</v>
@@ -2027,7 +2006,7 @@
         <v>52</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D52" s="9">
         <v>425</v>
@@ -2041,7 +2020,7 @@
         <v>53</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D53" s="9">
         <v>459</v>
@@ -2055,7 +2034,7 @@
         <v>54</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D54" s="9">
         <v>472</v>
@@ -2069,7 +2048,7 @@
         <v>55</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D55" s="9">
         <v>490</v>
@@ -2083,7 +2062,7 @@
         <v>56</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D56" s="9">
         <v>501</v>
@@ -2111,7 +2090,7 @@
         <v>58</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D58" s="9">
         <v>513</v>
@@ -2125,7 +2104,7 @@
         <v>59</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D59" s="9">
         <v>517</v>
@@ -2139,7 +2118,7 @@
         <v>60</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="D60" s="9">
         <v>520</v>
@@ -2153,7 +2132,7 @@
         <v>61</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D61" s="9">
         <v>521</v>
@@ -2167,7 +2146,7 @@
         <v>62</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D62" s="9">
         <v>523</v>
@@ -2181,7 +2160,7 @@
         <v>63</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D63" s="9">
         <v>526</v>
@@ -2195,7 +2174,7 @@
         <v>64</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D64" s="9">
         <v>531</v>
@@ -2209,7 +2188,7 @@
         <v>65</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D65" s="9">
         <v>535</v>
@@ -2223,7 +2202,7 @@
         <v>66</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D66" s="9">
         <v>536</v>
@@ -2251,7 +2230,7 @@
         <v>68</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D68" s="9">
         <v>547</v>
@@ -2265,7 +2244,7 @@
         <v>69</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D69" s="9">
         <v>548</v>
@@ -2279,7 +2258,7 @@
         <v>70</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D70" s="9">
         <v>562</v>
@@ -2293,7 +2272,7 @@
         <v>71</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D71" s="9">
         <v>564</v>
@@ -2307,7 +2286,7 @@
         <v>72</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D72" s="9">
         <v>566</v>
@@ -2321,7 +2300,7 @@
         <v>73</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D73" s="9">
         <v>567</v>
@@ -2349,7 +2328,7 @@
         <v>75</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>159</v>
@@ -2363,7 +2342,7 @@
         <v>76</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>256</v>
+        <v>278</v>
       </c>
       <c r="D76" s="9" t="s">
         <v>160</v>
@@ -2377,7 +2356,7 @@
         <v>77</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D77" s="9" t="s">
         <v>161</v>
@@ -2391,7 +2370,7 @@
         <v>78</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>162</v>
@@ -2405,7 +2384,7 @@
         <v>79</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>163</v>
@@ -2433,7 +2412,7 @@
         <v>81</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>164</v>
@@ -2447,7 +2426,7 @@
         <v>82</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>165</v>
@@ -2461,7 +2440,7 @@
         <v>83</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>110</v>
@@ -2475,7 +2454,7 @@
         <v>84</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>166</v>
@@ -2489,7 +2468,7 @@
         <v>85</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>167</v>
@@ -2503,7 +2482,7 @@
         <v>86</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D86" s="9">
         <v>122</v>
@@ -2517,7 +2496,7 @@
         <v>87</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D87" s="9" t="s">
         <v>168</v>
@@ -2531,7 +2510,7 @@
         <v>88</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="D88" s="9" t="s">
         <v>169</v>
@@ -2545,7 +2524,7 @@
         <v>89</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D89" s="9" t="s">
         <v>170</v>
@@ -2559,7 +2538,7 @@
         <v>90</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D90" s="9" t="s">
         <v>171</v>
@@ -2573,7 +2552,7 @@
         <v>91</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="D91" s="9" t="s">
         <v>172</v>
@@ -2601,7 +2580,7 @@
         <v>93</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D93" s="9">
         <v>129</v>
@@ -2615,7 +2594,7 @@
         <v>94</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D94" s="9" t="s">
         <v>174</v>
@@ -2629,7 +2608,7 @@
         <v>95</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="D95" s="9" t="s">
         <v>175</v>
@@ -2643,7 +2622,7 @@
         <v>96</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D96" s="9" t="s">
         <v>176</v>
@@ -2657,7 +2636,7 @@
         <v>97</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D97" s="9" t="s">
         <v>177</v>
@@ -2671,7 +2650,7 @@
         <v>98</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="D98" s="9" t="s">
         <v>178</v>
@@ -2685,7 +2664,7 @@
         <v>99</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="D99" s="9" t="s">
         <v>179</v>
@@ -2699,7 +2678,7 @@
         <v>100</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D100" s="9" t="s">
         <v>181</v>
@@ -2713,7 +2692,7 @@
         <v>101</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>150</v>
@@ -2830,6 +2809,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008E73E415D080F44580FCF4BB7CA46D35" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="829cabdc2c80afdf281131c4dae820fb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48c5b5cd9b8d25ff6dd15848836f4270" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2961,15 +2949,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2980,6 +2959,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B7BB02-ECBA-49DA-99C9-4485162341EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A542E15-BC5D-4020-AED2-89FFACD3984E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2997,16 +2986,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B7BB02-ECBA-49DA-99C9-4485162341EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80E25383-8D74-4FB8-BE33-82F272C93267}">
   <ds:schemaRefs>

</xml_diff>